<commit_message>
Ejercicio 1 listorti en excel
</commit_message>
<xml_diff>
--- a/Mediciones.xlsx
+++ b/Mediciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3E461B-89C1-4CD0-8CF0-9B3C38AA10DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D8039A-64C4-40C8-9F44-8DB3DB148410}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="34">
   <si>
     <t>Circuito</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>Núcleo 1: maciso (homogeneo) de hierro (207)</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poca diferencia entre la resistencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y la reactancia, por eso cos(phi) </t>
+  </si>
+  <si>
+    <t>da igual en A y C</t>
   </si>
 </sst>
 </file>
@@ -140,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +195,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -287,11 +305,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -358,6 +413,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -640,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,30 +901,187 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="N7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="36">
+        <v>22.6</v>
+      </c>
+      <c r="P7" s="37" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
+      <c r="N9" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="29"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5">
+        <f>28.7*0.25</f>
+        <v>7.1749999999999998</v>
+      </c>
+      <c r="C10" s="5">
+        <f>0.55/2</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D10" s="5">
+        <v>99</v>
+      </c>
+      <c r="E10" s="6">
+        <f>$B10</f>
+        <v>7.1749999999999998</v>
+      </c>
+      <c r="F10" s="6">
+        <f>SQRT($G10^2-$E10^2)</f>
+        <v>26.262520823409165</v>
+      </c>
+      <c r="G10" s="6">
+        <f>$C10*$D10</f>
+        <v>27.225000000000001</v>
+      </c>
+      <c r="H10" s="6">
+        <f>$E10/$G10</f>
+        <v>0.26354453627180896</v>
+      </c>
       <c r="K10" s="2"/>
+      <c r="N10" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="32"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5">
+        <f>31*0.25</f>
+        <v>7.75</v>
+      </c>
+      <c r="C11" s="5">
+        <f>0.365</f>
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="D11" s="5">
+        <v>98.5</v>
+      </c>
+      <c r="E11" s="6">
+        <f>$B11</f>
+        <v>7.75</v>
+      </c>
+      <c r="F11" s="6">
+        <f>SQRT($G11^2-$E11^2)</f>
+        <v>35.10726073407038</v>
+      </c>
+      <c r="G11" s="6">
+        <f>$C11*$D11</f>
+        <v>35.952500000000001</v>
+      </c>
+      <c r="H11" s="6">
+        <f>$E11/$G11</f>
+        <v>0.21556220012516514</v>
+      </c>
+      <c r="N11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="35"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5">
+        <f>92*0.25</f>
+        <v>23</v>
+      </c>
+      <c r="C12" s="5">
+        <f>0.918</f>
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="D12" s="5">
+        <v>95.1</v>
+      </c>
+      <c r="E12" s="6">
+        <f>$B12</f>
+        <v>23</v>
+      </c>
+      <c r="F12" s="6">
+        <f>SQRT($G12^2-$E12^2)</f>
+        <v>84.217600792470932</v>
+      </c>
+      <c r="G12" s="6">
+        <f>$C12*$D12</f>
+        <v>87.3018</v>
+      </c>
+      <c r="H12" s="6">
+        <f>$E12/$G12</f>
+        <v>0.2634539035850349</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="N11:Q11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="N3:Q3"/>

</xml_diff>

<commit_message>
FALTAN: conclusión del ejercicio 2, del 4 y comparar resultados del circuito RLC del 4 con 3 Y HACER QUE DE CON SENTIDO
</commit_message>
<xml_diff>
--- a/Mediciones.xlsx
+++ b/Mediciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6545862-1B8E-4912-908B-E949AD0E73EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE910940-4ABB-4E50-8411-F746C978465D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
   <si>
     <t>Circuito</t>
   </si>
@@ -141,12 +141,21 @@
   </si>
   <si>
     <t>Medición</t>
+  </si>
+  <si>
+    <t>phi (rad)</t>
+  </si>
+  <si>
+    <t>phi (grados)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -214,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -318,19 +327,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -358,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -391,19 +387,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -431,9 +431,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,7 +463,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -752,25 +750,28 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="I2" sqref="I2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -797,12 +798,18 @@
       <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="I2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="30"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -835,12 +842,20 @@
         <f>$E3/$G3</f>
         <v>0.26496116948378257</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="I3" s="14">
+        <f>ACOS(H3)</f>
+        <v>1.3026326744935872</v>
+      </c>
+      <c r="J3" s="14">
+        <f>180*I3/(2*PI())</f>
+        <v>37.317677252160657</v>
+      </c>
+      <c r="N3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="33"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -873,12 +888,20 @@
         <f t="shared" ref="H4:H5" si="3">$E4/$G4</f>
         <v>0.22033803759692083</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="I4" s="14">
+        <f t="shared" ref="I4:I5" si="4">ACOS(H4)</f>
+        <v>1.3486353151827004</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" ref="J4:J5" si="5">180*I4/(2*PI())</f>
+        <v>38.635555831132145</v>
+      </c>
+      <c r="N4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="36"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -910,6 +933,14 @@
       <c r="H5" s="6">
         <f t="shared" si="3"/>
         <v>0.26267624728850325</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" si="4"/>
+        <v>1.3050015201360681</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="5"/>
+        <v>37.385539680976713</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -930,18 +961,18 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -969,15 +1000,19 @@
       <c r="H9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="I9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="K9" s="2"/>
-      <c r="N9" s="17" t="s">
+      <c r="N9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="19"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="21"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1010,13 +1045,21 @@
         <f>$E10/$G10</f>
         <v>0.26354453627180896</v>
       </c>
+      <c r="I10" s="14">
+        <f>ACOS(H10)</f>
+        <v>1.3041015202827992</v>
+      </c>
+      <c r="J10" s="14">
+        <f>180*I10/(2*PI())</f>
+        <v>37.359756584399364</v>
+      </c>
       <c r="K10" s="2"/>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="22"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="24"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1049,12 +1092,20 @@
         <f>$E11/$G11</f>
         <v>0.21556220012516514</v>
       </c>
-      <c r="N11" s="23" t="s">
+      <c r="I11" s="14">
+        <f t="shared" ref="I11:I12" si="6">ACOS(H11)</f>
+        <v>1.353528797898006</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" ref="J11:J12" si="7">180*I11/(2*PI())</f>
+        <v>38.775743784485755</v>
+      </c>
+      <c r="N11" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="25"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="27"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1087,14 +1138,22 @@
         <f>$E12/$G12</f>
         <v>0.2634539035850349</v>
       </c>
+      <c r="I12" s="14">
+        <f t="shared" si="6"/>
+        <v>1.3041954733062036</v>
+      </c>
+      <c r="J12" s="14">
+        <f t="shared" si="7"/>
+        <v>37.362448140256141</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A8:J8"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
@@ -1106,41 +1165,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA547B70-7A50-49C7-9348-70470A4155B1}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A16" sqref="A16:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="11" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="P1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1165,20 +1227,26 @@
       <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1210,30 +1278,38 @@
         <f>E3/G3</f>
         <v>0.99352839303618623</v>
       </c>
-      <c r="I3" s="6">
-        <f>(D3^2)/(2*PI()*$O$3*($F3-$E3*$O$6/ABS($O$4)))</f>
-        <v>-3.0061605425824833</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="14">
+        <f>ACOS(H3)</f>
+        <v>0.11382969136405419</v>
+      </c>
+      <c r="J3" s="14">
+        <f>180*I3/(2*PI())</f>
+        <v>3.2609804492185299</v>
+      </c>
+      <c r="K3" s="6">
+        <f>(D3^2)/(2*PI()*$Q$3*($F3-$E3*$Q$6/$Q$4))</f>
+        <v>-3.0061605425824873</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="8">
+      <c r="M3" s="8">
         <v>16.7</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="3">
+      <c r="Q3" s="3">
         <v>50</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1265,30 +1341,38 @@
         <f t="shared" ref="H4:H5" si="2">E4/G4</f>
         <v>8.8028169014084501E-2</v>
       </c>
-      <c r="I4" s="6">
-        <f t="shared" ref="I4:I5" si="3">(D4^2)/(2*PI()*$O$3*($F4-$E4*$O$6/ABS($O$4)))</f>
-        <v>0.63206799416828929</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="14">
+        <f t="shared" ref="I4:I5" si="3">ACOS(H4)</f>
+        <v>1.4826540717377461</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" ref="J4:J5" si="4">180*I4/(2*PI())</f>
+        <v>42.474910394229816</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" ref="K4:K5" si="5">(D4^2)/(2*PI()*$Q$3*($F4-$E4*$Q$6/$Q$4))</f>
+        <v>0.63206799416828907</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="8">
+      <c r="M4" s="8">
         <v>16</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="3">
-        <v>-0.9</v>
-      </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="R4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1320,34 +1404,42 @@
         <f t="shared" si="2"/>
         <v>0.74068332342884702</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="14">
         <f t="shared" si="3"/>
-        <v>1.5487088338183987</v>
-      </c>
-      <c r="N5" s="8" t="s">
+        <v>0.73670946700186102</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="4"/>
+        <v>21.105171593269514</v>
+      </c>
+      <c r="K5" s="6">
+        <f t="shared" si="5"/>
+        <v>1.5487088338183972</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="3">
-        <f>ACOS(O4)</f>
-        <v>2.6905658417935303</v>
-      </c>
-      <c r="P5" s="8" t="s">
+      <c r="Q5" s="3">
+        <f>ACOS(Q4)</f>
+        <v>0.45102681179626236</v>
+      </c>
+      <c r="R5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N6" s="8" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="3">
-        <f>SIN(O5)</f>
-        <v>0.43588989435406778</v>
-      </c>
-      <c r="P6" s="8" t="s">
+      <c r="Q6" s="3">
+        <f>SIN(Q5)</f>
+        <v>0.43588989435406728</v>
+      </c>
+      <c r="R6" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1357,27 +1449,28 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1402,9 +1495,14 @@
       <c r="H10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1422,7 +1520,7 @@
         <v>89</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" ref="F11" si="4">SQRT(G11^2-E11^2)</f>
+        <f t="shared" ref="F11" si="6">SQRT(G11^2-E11^2)</f>
         <v>40.592516551699518</v>
       </c>
       <c r="G11" s="6">
@@ -1430,20 +1528,28 @@
         <v>97.82</v>
       </c>
       <c r="H11" s="6">
-        <f t="shared" ref="H11" si="5">E11/G11</f>
+        <f t="shared" ref="H11" si="7">E11/G11</f>
         <v>0.9098343896953589</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="14">
+        <f>ACOS(H11)</f>
+        <v>0.42791152805043664</v>
+      </c>
+      <c r="J11" s="14">
+        <f>180*I11/(2*PI())</f>
+        <v>12.258762281141978</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="8">
+      <c r="L11" s="8">
         <v>24</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="M11" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1461,7 +1567,7 @@
         <v>87</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" ref="F12" si="6">SQRT(G12^2-E12^2)</f>
+        <f t="shared" ref="F12" si="8">SQRT(G12^2-E12^2)</f>
         <v>77.960967156648337</v>
       </c>
       <c r="G12" s="6">
@@ -1469,24 +1575,48 @@
         <v>116.82000000000001</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" ref="H12" si="7">E12/G12</f>
+        <f t="shared" ref="H12" si="9">E12/G12</f>
         <v>0.74473549049820231</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="14">
+        <f t="shared" ref="I12" si="10">ACOS(H12)</f>
+        <v>0.73065792558985365</v>
+      </c>
+      <c r="J12" s="14">
+        <f t="shared" ref="J12" si="11">180*I12/(2*PI())</f>
+        <v>20.93180770204118</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="8">
+      <c r="L12" s="8">
         <v>16</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="M12" s="8" t="s">
         <v>35</v>
       </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J14" s="16"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
que se yo, yo pusheo
</commit_message>
<xml_diff>
--- a/Mediciones.xlsx
+++ b/Mediciones.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244FB694-EC63-440F-B1EB-05BC986CD431}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1C5161-E95B-407E-A1D8-3574F82A2EFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17235" yWindow="7110" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejercicio 1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -414,6 +414,15 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,16 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -788,18 +788,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -832,12 +832,12 @@
       <c r="J2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -878,12 +878,12 @@
         <f>180*I3/(2*PI())</f>
         <v>37.317677252160657</v>
       </c>
-      <c r="N3" s="31" t="s">
+      <c r="N3" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="33"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="36"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -924,12 +924,12 @@
         <f t="shared" ref="J4:J5" si="5">180*I4/(2*PI())</f>
         <v>38.635555831132145</v>
       </c>
-      <c r="N4" s="34" t="s">
+      <c r="N4" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="36"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="39"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -989,18 +989,18 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1035,12 +1035,12 @@
         <v>39</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="N9" s="19" t="s">
+      <c r="N9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="21"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="24"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1082,12 +1082,12 @@
         <v>37.359756584399364</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="24"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1128,12 +1128,12 @@
         <f t="shared" ref="J11:J12" si="7">180*I11/(2*PI())</f>
         <v>38.775743784485755</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="27"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="30"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1210,24 +1210,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="42" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1313,19 +1313,19 @@
         <f>180*I3/(2*PI())</f>
         <v>3.2609804492185299</v>
       </c>
-      <c r="K3" s="41">
+      <c r="K3" s="18">
         <f>(D3^2)/F3</f>
         <v>3056.5019261816105</v>
       </c>
-      <c r="L3" s="41">
+      <c r="L3" s="18">
         <f>G3*$B$21</f>
         <v>23.910740154792361</v>
       </c>
-      <c r="M3" s="41">
+      <c r="M3" s="18">
         <f>K3-L3</f>
         <v>3032.5911860268184</v>
       </c>
-      <c r="N3" s="43">
+      <c r="N3" s="19">
         <f>1/(2*PI()*$B$18*M3)</f>
         <v>1.0496300577883949E-6</v>
       </c>
@@ -1379,19 +1379,19 @@
         <f t="shared" ref="J4:J5" si="4">180*I4/(2*PI())</f>
         <v>42.474910394229816</v>
       </c>
-      <c r="K4" s="41">
+      <c r="K4" s="18">
         <f>(D4^2)/F4</f>
         <v>190.07119241793242</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="18">
         <f>G4*$B$21</f>
         <v>46.422273748708164</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="18">
         <f t="shared" ref="M4:M5" si="5">K4-L4</f>
         <v>143.64891866922426</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="19">
         <f>1/(2*PI()*$B$18*M4)</f>
         <v>2.2158877987571393E-5</v>
       </c>
@@ -1445,19 +1445,19 @@
         <f t="shared" si="4"/>
         <v>21.105171593269514</v>
       </c>
-      <c r="K5" s="41">
+      <c r="K5" s="18">
         <f>(D5^2)/F5</f>
         <v>226.7578285297173</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="18">
         <f>G5*$B$21</f>
         <v>50.610739743556394</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="18">
         <f t="shared" si="5"/>
         <v>176.14708878616091</v>
       </c>
-      <c r="N5" s="43">
+      <c r="N5" s="19">
         <f>1/(2*PI()*$B$18*M5)</f>
         <v>1.8070686741250239E-5</v>
       </c>
@@ -1478,18 +1478,18 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
       <c r="K9" s="2"/>
       <c r="N9" s="2"/>
     </row>
@@ -1627,16 +1627,16 @@
       <c r="J14" s="15"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -1649,7 +1649,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="16"/>
-      <c r="M17" s="39"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1662,7 +1662,7 @@
         <v>18</v>
       </c>
       <c r="F18" s="16"/>
-      <c r="M18" s="39"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -1675,7 +1675,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="16"/>
-      <c r="M19" s="39"/>
+      <c r="M19" s="17"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">

</xml_diff>